<commit_message>
Update blank input sheet.
</commit_message>
<xml_diff>
--- a/xlsx/hfc_inputs_blank.xlsx
+++ b/xlsx/hfc_inputs_blank.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cboyer.IPA\Desktop\high-frequency-checks\xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cboyer.IPA\Desktop\high-frequency-checks\exercise\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11970" windowHeight="4650" firstSheet="4" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11970" windowHeight="4650" firstSheet="2" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="1. incomplete" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="29">
   <si>
     <t>variable</t>
   </si>
@@ -63,9 +63,6 @@
     <t>surveystart</t>
   </si>
   <si>
-    <t>iqr_multiplier</t>
-  </si>
-  <si>
     <t>submission_date</t>
   </si>
   <si>
@@ -90,9 +87,6 @@
     <t>exclude_variable</t>
   </si>
   <si>
-    <t>output_variable</t>
-  </si>
-  <si>
     <t>coming soon</t>
   </si>
   <si>
@@ -106,6 +100,24 @@
   </si>
   <si>
     <t>if_condition</t>
+  </si>
+  <si>
+    <t>complete_percent</t>
+  </si>
+  <si>
+    <t>keep</t>
+  </si>
+  <si>
+    <t>keep_current</t>
+  </si>
+  <si>
+    <t>keep_master</t>
+  </si>
+  <si>
+    <t>multiplier</t>
+  </si>
+  <si>
+    <t>other_variable</t>
   </si>
 </sst>
 </file>
@@ -521,13 +533,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>57150</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>942975</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
@@ -605,13 +617,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>57150</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>180975</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>962025</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
@@ -680,13 +692,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>57150</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>962025</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
@@ -752,16 +764,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>962025</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>971550</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -770,7 +782,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6962775" y="2876550"/>
+          <a:off x="6972300" y="4000500"/>
           <a:ext cx="3667125" cy="609600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -807,7 +819,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1100" b="1"/>
-            <a:t>output_variable</a:t>
+            <a:t>keep</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="1100" b="1" baseline="0"/>
         </a:p>
@@ -840,16 +852,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>962025</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>971550</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -858,7 +870,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6962775" y="3571875"/>
+          <a:off x="6972300" y="4695825"/>
           <a:ext cx="3667125" cy="609600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -903,6 +915,247 @@
           <a:r>
             <a:rPr lang="en-US" sz="1100" b="0" baseline="0"/>
             <a:t>This column is not used by Stata, rather it is included for the user's convenience to keep notes about inputs</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="0"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1238250</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="8" name="Group 7"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="11191875" y="314325"/>
+          <a:ext cx="1095375" cy="723900"/>
+          <a:chOff x="10401300" y="1847850"/>
+          <a:chExt cx="1095375" cy="723900"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="9" name="TextBox 8"/>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="10401300" y="1847850"/>
+            <a:ext cx="1095375" cy="723900"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="lt1"/>
+          </a:solidFill>
+          <a:ln w="9525" cmpd="sng">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100" b="1"/>
+              <a:t>Required</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:endParaRPr lang="en-US" sz="1100" b="1"/>
+          </a:p>
+          <a:p>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100" b="1"/>
+              <a:t>Optional</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="10" name="Rectangle 9"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm flipV="1">
+            <a:off x="11134727" y="1933575"/>
+            <a:ext cx="209548" cy="228600"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:srgbClr val="92D050"/>
+          </a:solidFill>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="13" name="Rectangle 12"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm flipV="1">
+            <a:off x="11134727" y="2266950"/>
+            <a:ext cx="209548" cy="228600"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:srgbClr val="FFC000"/>
+          </a:solidFill>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>57149</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>962025</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>161924</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="14" name="TextBox 13"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6962775" y="2914649"/>
+          <a:ext cx="3667125" cy="866775"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="92D050"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1"/>
+            <a:t>complete_percent</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="1" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" baseline="0"/>
+            <a:t>This column specifies a minimum non-missing percentage for each interview. Any interview that falls below this threshold will be flagged as incomplete and included in the output.</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="1100" b="0"/>
         </a:p>
@@ -1478,7 +1731,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1100" b="1"/>
-            <a:t>output_variable</a:t>
+            <a:t>keep</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="1100" b="1" baseline="0"/>
         </a:p>
@@ -1579,6 +1832,175 @@
         </a:p>
       </xdr:txBody>
     </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>1238250</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="12" name="Group 11"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="13954125" y="590550"/>
+          <a:ext cx="1095375" cy="723900"/>
+          <a:chOff x="10401300" y="1847850"/>
+          <a:chExt cx="1095375" cy="723900"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="13" name="TextBox 12"/>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="10401300" y="1847850"/>
+            <a:ext cx="1095375" cy="723900"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="lt1"/>
+          </a:solidFill>
+          <a:ln w="9525" cmpd="sng">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100" b="1"/>
+              <a:t>Required</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:endParaRPr lang="en-US" sz="1100" b="1"/>
+          </a:p>
+          <a:p>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100" b="1"/>
+              <a:t>Optional</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="14" name="Rectangle 13"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm flipV="1">
+            <a:off x="11134727" y="1933575"/>
+            <a:ext cx="209548" cy="228600"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:srgbClr val="92D050"/>
+          </a:solidFill>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="15" name="Rectangle 14"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm flipV="1">
+            <a:off x="11134727" y="2266950"/>
+            <a:ext cx="209548" cy="228600"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:srgbClr val="FFC000"/>
+          </a:solidFill>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -1660,7 +2082,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1100" b="0" i="1" baseline="0"/>
-            <a:t>This check verifies whether certain continuous variables contain outliers, where an outlier is defined to be a certain multiple of the IQR.</a:t>
+            <a:t>This check verifies whether certain continuous variables contain outliers, where an outlier is defined to be a certain multiple of the IQR or SD (Note: IQR or SD is specified in the master_check file).</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -1802,14 +2224,14 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1100" b="1"/>
-            <a:t>iqr_multiplier</a:t>
+            <a:t>multiplier</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="1100" b="1" baseline="0"/>
         </a:p>
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1100" b="0" baseline="0"/>
-            <a:t>This column specifies the multiple of the interquartile range that signifies an outlier.</a:t>
+            <a:t>This column specifies the multiple of the interquartile range or standard deviation that signifies an outlier.</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="1100" b="0"/>
         </a:p>
@@ -1874,7 +2296,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1100" b="1"/>
-            <a:t>output_variable</a:t>
+            <a:t>keep</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="1100" b="1" baseline="0"/>
         </a:p>
@@ -1975,6 +2397,175 @@
         </a:p>
       </xdr:txBody>
     </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1238250</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="7" name="Group 6"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="9810750" y="361950"/>
+          <a:ext cx="1095375" cy="723900"/>
+          <a:chOff x="10401300" y="1847850"/>
+          <a:chExt cx="1095375" cy="723900"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="8" name="TextBox 7"/>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="10401300" y="1847850"/>
+            <a:ext cx="1095375" cy="723900"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="lt1"/>
+          </a:solidFill>
+          <a:ln w="9525" cmpd="sng">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100" b="1"/>
+              <a:t>Required</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:endParaRPr lang="en-US" sz="1100" b="1"/>
+          </a:p>
+          <a:p>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100" b="1"/>
+              <a:t>Optional</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="9" name="Rectangle 8"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm flipV="1">
+            <a:off x="11134727" y="1933575"/>
+            <a:ext cx="209548" cy="228600"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:srgbClr val="92D050"/>
+          </a:solidFill>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="10" name="Rectangle 9"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm flipV="1">
+            <a:off x="11134727" y="2266950"/>
+            <a:ext cx="209548" cy="228600"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:srgbClr val="FFC000"/>
+          </a:solidFill>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -2432,6 +3023,175 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>1247775</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="8" name="Group 7"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="12582525" y="495300"/>
+          <a:ext cx="1095375" cy="723900"/>
+          <a:chOff x="10401300" y="1847850"/>
+          <a:chExt cx="1095375" cy="723900"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="9" name="TextBox 8"/>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="10401300" y="1847850"/>
+            <a:ext cx="1095375" cy="723900"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="lt1"/>
+          </a:solidFill>
+          <a:ln w="9525" cmpd="sng">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100" b="1"/>
+              <a:t>Required</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:endParaRPr lang="en-US" sz="1100" b="1"/>
+          </a:p>
+          <a:p>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100" b="1"/>
+              <a:t>Optional</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="10" name="Rectangle 9"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm flipV="1">
+            <a:off x="11134727" y="1933575"/>
+            <a:ext cx="209548" cy="228600"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:srgbClr val="92D050"/>
+          </a:solidFill>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="11" name="Rectangle 10"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm flipV="1">
+            <a:off x="11134727" y="2266950"/>
+            <a:ext cx="209548" cy="228600"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:srgbClr val="FFC000"/>
+          </a:solidFill>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2730,7 +3490,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1100" b="1"/>
-            <a:t>output_variable</a:t>
+            <a:t>keep</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="1100" b="1" baseline="0"/>
         </a:p>
@@ -2831,6 +3591,175 @@
         </a:p>
       </xdr:txBody>
     </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1238250</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="4" name="Group 3"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="9810750" y="323850"/>
+          <a:ext cx="1095375" cy="723900"/>
+          <a:chOff x="10401300" y="1847850"/>
+          <a:chExt cx="1095375" cy="723900"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="3" name="TextBox 2"/>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="10401300" y="1847850"/>
+            <a:ext cx="1095375" cy="723900"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="lt1"/>
+          </a:solidFill>
+          <a:ln w="9525" cmpd="sng">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100" b="1"/>
+              <a:t>Required</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:endParaRPr lang="en-US" sz="1100" b="1"/>
+          </a:p>
+          <a:p>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100" b="1"/>
+              <a:t>Optional</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="2" name="Rectangle 1"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm flipV="1">
+            <a:off x="11134727" y="1933575"/>
+            <a:ext cx="209548" cy="228600"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:srgbClr val="92D050"/>
+          </a:solidFill>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="13" name="Rectangle 12"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm flipV="1">
+            <a:off x="11134727" y="2266950"/>
+            <a:ext cx="209548" cy="228600"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:srgbClr val="FFC000"/>
+          </a:solidFill>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -3126,7 +4055,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1100" b="1"/>
-            <a:t>output_variable</a:t>
+            <a:t>keep</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="1100" b="1" baseline="0"/>
         </a:p>
@@ -3227,6 +4156,175 @@
         </a:p>
       </xdr:txBody>
     </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1238250</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="12" name="Group 11"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="9810750" y="304800"/>
+          <a:ext cx="1095375" cy="723900"/>
+          <a:chOff x="10401300" y="1847850"/>
+          <a:chExt cx="1095375" cy="723900"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="13" name="TextBox 12"/>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="10401300" y="1847850"/>
+            <a:ext cx="1095375" cy="723900"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="lt1"/>
+          </a:solidFill>
+          <a:ln w="9525" cmpd="sng">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100" b="1"/>
+              <a:t>Required</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:endParaRPr lang="en-US" sz="1100" b="1"/>
+          </a:p>
+          <a:p>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100" b="1"/>
+              <a:t>Optional</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="14" name="Rectangle 13"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm flipV="1">
+            <a:off x="11134727" y="1933575"/>
+            <a:ext cx="209548" cy="228600"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:srgbClr val="92D050"/>
+          </a:solidFill>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="15" name="Rectangle 14"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm flipV="1">
+            <a:off x="11134727" y="2266950"/>
+            <a:ext cx="209548" cy="228600"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:srgbClr val="FFC000"/>
+          </a:solidFill>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -3448,7 +4546,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1100" b="1"/>
-            <a:t>output_variable</a:t>
+            <a:t>keep</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="1100" b="1" baseline="0"/>
         </a:p>
@@ -3551,6 +4649,175 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1247775</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="7" name="Group 6"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="8439150" y="304800"/>
+          <a:ext cx="1095375" cy="723900"/>
+          <a:chOff x="10401300" y="1847850"/>
+          <a:chExt cx="1095375" cy="723900"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="8" name="TextBox 7"/>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="10401300" y="1847850"/>
+            <a:ext cx="1095375" cy="723900"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="lt1"/>
+          </a:solidFill>
+          <a:ln w="9525" cmpd="sng">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100" b="1"/>
+              <a:t>Required</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:endParaRPr lang="en-US" sz="1100" b="1"/>
+          </a:p>
+          <a:p>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100" b="1"/>
+              <a:t>Optional</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="9" name="Rectangle 8"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm flipV="1">
+            <a:off x="11134727" y="1933575"/>
+            <a:ext cx="209548" cy="228600"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:srgbClr val="92D050"/>
+          </a:solidFill>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="10" name="Rectangle 9"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm flipV="1">
+            <a:off x="11134727" y="2266950"/>
+            <a:ext cx="209548" cy="228600"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:srgbClr val="FFC000"/>
+          </a:solidFill>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -3558,13 +4825,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>47625</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>933450</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
@@ -3657,13 +4924,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>47625</xdr:colOff>
       <xdr:row>9</xdr:row>
       <xdr:rowOff>76201</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>952500</xdr:colOff>
       <xdr:row>12</xdr:row>
       <xdr:rowOff>114301</xdr:rowOff>
@@ -3732,16 +4999,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>190499</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>962025</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -3750,7 +5017,103 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5581650" y="2476500"/>
+          <a:off x="5581650" y="2476499"/>
+          <a:ext cx="3667125" cy="790576"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFC000"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1"/>
+            <a:t>keep_current</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="1" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" baseline="0"/>
+            <a:t>This column specifies additional variable values from the </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" baseline="0"/>
+            <a:t>data set in memory </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" baseline="0"/>
+            <a:t>to display in the output file. By default </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" baseline="0"/>
+            <a:t>id </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" baseline="0"/>
+            <a:t>and </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" baseline="0"/>
+            <a:t>enumerator</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" baseline="0"/>
+            <a:t> are displayed.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="0"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>962025</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="TextBox 4"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5581650" y="4038600"/>
           <a:ext cx="3667125" cy="609600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3787,30 +5150,14 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1100" b="1"/>
-            <a:t>output_variable</a:t>
+            <a:t>notes</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="1100" b="1" baseline="0"/>
         </a:p>
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1100" b="0" baseline="0"/>
-            <a:t>This column specifies additional variable values to display in the output file. By default </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1" baseline="0"/>
-            <a:t>id </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" baseline="0"/>
-            <a:t>and </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1" baseline="0"/>
-            <a:t>enumerator</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" baseline="0"/>
-            <a:t> are displayed.</a:t>
+            <a:t>This column is not used by Stata, rather it is included for the user's convenience to keep notes about inputs</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="1100" b="0"/>
         </a:p>
@@ -3820,26 +5167,195 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1238250</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="6" name="Group 5"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="9810750" y="495300"/>
+          <a:ext cx="1095375" cy="723900"/>
+          <a:chOff x="10401300" y="1847850"/>
+          <a:chExt cx="1095375" cy="723900"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="7" name="TextBox 6"/>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="10401300" y="1847850"/>
+            <a:ext cx="1095375" cy="723900"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="lt1"/>
+          </a:solidFill>
+          <a:ln w="9525" cmpd="sng">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100" b="1"/>
+              <a:t>Required</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:endParaRPr lang="en-US" sz="1100" b="1"/>
+          </a:p>
+          <a:p>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100" b="1"/>
+              <a:t>Optional</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="8" name="Rectangle 7"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm flipV="1">
+            <a:off x="11134727" y="1933575"/>
+            <a:ext cx="209548" cy="228600"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:srgbClr val="92D050"/>
+          </a:solidFill>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="9" name="Rectangle 8"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm flipV="1">
+            <a:off x="11134727" y="2266950"/>
+            <a:ext cx="209548" cy="228600"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:srgbClr val="FFC000"/>
+          </a:solidFill>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>95249</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>962025</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5" name="TextBox 4"/>
+        <xdr:cNvPr id="10" name="TextBox 9"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5581650" y="3181350"/>
-          <a:ext cx="3667125" cy="609600"/>
+          <a:off x="5581650" y="3333749"/>
+          <a:ext cx="3667125" cy="609601"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3875,14 +5391,22 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1100" b="1"/>
-            <a:t>notes</a:t>
+            <a:t>keep_master</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="1100" b="1" baseline="0"/>
         </a:p>
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1100" b="0" baseline="0"/>
-            <a:t>This column is not used by Stata, rather it is included for the user's convenience to keep notes about inputs</a:t>
+            <a:t>This column specifies additional variable values from the </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" baseline="0"/>
+            <a:t>master tracking list </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" baseline="0"/>
+            <a:t>set to display in the output file. </a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="1100" b="0"/>
         </a:p>
@@ -4180,7 +5704,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1100" b="1"/>
-            <a:t>output_variable</a:t>
+            <a:t>keep</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="1100" b="1" baseline="0"/>
         </a:p>
@@ -4354,6 +5878,175 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1247775</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="8" name="Group 7"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="11201400" y="381000"/>
+          <a:ext cx="1095375" cy="723900"/>
+          <a:chOff x="10401300" y="1847850"/>
+          <a:chExt cx="1095375" cy="723900"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="9" name="TextBox 8"/>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="10401300" y="1847850"/>
+            <a:ext cx="1095375" cy="723900"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="lt1"/>
+          </a:solidFill>
+          <a:ln w="9525" cmpd="sng">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100" b="1"/>
+              <a:t>Required</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:endParaRPr lang="en-US" sz="1100" b="1"/>
+          </a:p>
+          <a:p>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100" b="1"/>
+              <a:t>Optional</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="10" name="Rectangle 9"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm flipV="1">
+            <a:off x="11134727" y="1933575"/>
+            <a:ext cx="209548" cy="228600"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:srgbClr val="92D050"/>
+          </a:solidFill>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="11" name="Rectangle 10"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm flipV="1">
+            <a:off x="11134727" y="2266950"/>
+            <a:ext cx="209548" cy="228600"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:srgbClr val="FFC000"/>
+          </a:solidFill>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -4361,13 +6054,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>57150</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>47624</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>942975</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
@@ -4445,13 +6138,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>57150</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>962025</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
@@ -4520,25 +6213,25 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>57150</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>962025</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="4" name="TextBox 3"/>
+        <xdr:cNvPr id="5" name="TextBox 4"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4200525" y="2857500"/>
+          <a:off x="2819400" y="2867025"/>
           <a:ext cx="3667125" cy="609600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -4575,30 +6268,14 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1100" b="1"/>
-            <a:t>output_variable</a:t>
+            <a:t>notes</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="1100" b="1" baseline="0"/>
         </a:p>
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1100" b="0" baseline="0"/>
-            <a:t>This column specifies additional variable values to display in the output file. By default </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1" baseline="0"/>
-            <a:t>id </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" baseline="0"/>
-            <a:t>and </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1" baseline="0"/>
-            <a:t>enumerator</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" baseline="0"/>
-            <a:t> are displayed.</a:t>
+            <a:t>This column is not used by Stata, rather it is included for the user's convenience to keep notes about inputs</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="1100" b="0"/>
         </a:p>
@@ -4608,74 +6285,171 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>962025</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:colOff>1228725</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="5" name="TextBox 4"/>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="6" name="Group 5"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="4200525" y="3562350"/>
-          <a:ext cx="3667125" cy="609600"/>
+          <a:off x="7038975" y="600075"/>
+          <a:ext cx="1095375" cy="723900"/>
+          <a:chOff x="10401300" y="1847850"/>
+          <a:chExt cx="1095375" cy="723900"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="FFC000"/>
-        </a:solidFill>
-        <a:ln w="9525" cmpd="sng">
-          <a:solidFill>
-            <a:schemeClr val="lt1">
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="7" name="TextBox 6"/>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="10401300" y="1847850"/>
+            <a:ext cx="1095375" cy="723900"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="lt1"/>
+          </a:solidFill>
+          <a:ln w="9525" cmpd="sng">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100" b="1"/>
+              <a:t>Required</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:endParaRPr lang="en-US" sz="1100" b="1"/>
+          </a:p>
+          <a:p>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100" b="1"/>
+              <a:t>Optional</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="8" name="Rectangle 7"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm flipV="1">
+            <a:off x="11134727" y="1933575"/>
+            <a:ext cx="209548" cy="228600"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:srgbClr val="92D050"/>
+          </a:solidFill>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
               <a:shade val="50000"/>
             </a:schemeClr>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1"/>
-            <a:t>notes</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1100" b="1" baseline="0"/>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" baseline="0"/>
-            <a:t>This column is not used by Stata, rather it is included for the user's convenience to keep notes about inputs</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1100" b="0"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="9" name="Rectangle 8"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm flipV="1">
+            <a:off x="11134727" y="2266950"/>
+            <a:ext cx="209548" cy="228600"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:srgbClr val="FFC000"/>
+          </a:solidFill>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -5223,7 +6997,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1100" b="1"/>
-            <a:t>output_variable</a:t>
+            <a:t>keep</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="1100" b="1" baseline="0"/>
         </a:p>
@@ -5326,6 +7100,175 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>1238250</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="10" name="Group 9"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="13954125" y="581025"/>
+          <a:ext cx="1095375" cy="723900"/>
+          <a:chOff x="10401300" y="1847850"/>
+          <a:chExt cx="1095375" cy="723900"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="11" name="TextBox 10"/>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="10401300" y="1847850"/>
+            <a:ext cx="1095375" cy="723900"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="lt1"/>
+          </a:solidFill>
+          <a:ln w="9525" cmpd="sng">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100" b="1"/>
+              <a:t>Required</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:endParaRPr lang="en-US" sz="1100" b="1"/>
+          </a:p>
+          <a:p>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100" b="1"/>
+              <a:t>Optional</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="12" name="Rectangle 11"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm flipV="1">
+            <a:off x="11134727" y="1933575"/>
+            <a:ext cx="209548" cy="228600"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:srgbClr val="92D050"/>
+          </a:solidFill>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="13" name="Rectangle 12"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm flipV="1">
+            <a:off x="11134727" y="2266950"/>
+            <a:ext cx="209548" cy="228600"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:srgbClr val="FFC000"/>
+          </a:solidFill>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -5333,13 +7276,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>47625</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>47624</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>933450</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>190499</xdr:rowOff>
@@ -5419,16 +7362,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>47625</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>952500</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -5438,7 +7381,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5572125" y="2181225"/>
-          <a:ext cx="3667125" cy="600075"/>
+          <a:ext cx="3667125" cy="657225"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5494,16 +7437,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>47625</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>952500</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -5512,7 +7455,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5572125" y="2867025"/>
+          <a:off x="5572125" y="3810000"/>
           <a:ext cx="3667125" cy="609600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -5549,7 +7492,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1100" b="1"/>
-            <a:t>output_variable</a:t>
+            <a:t>keep</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="1100" b="1" baseline="0"/>
         </a:p>
@@ -5582,16 +7525,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>47625</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>952500</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -5600,7 +7543,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5572125" y="3571875"/>
+          <a:off x="5572125" y="4514850"/>
           <a:ext cx="3667125" cy="609600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -5645,6 +7588,250 @@
           <a:r>
             <a:rPr lang="en-US" sz="1100" b="0" baseline="0"/>
             <a:t>This column is not used by Stata, rather it is included for the user's convenience to keep notes about inputs</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="0"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1238250</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="6" name="Group 5"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="9810750" y="695325"/>
+          <a:ext cx="1095375" cy="723900"/>
+          <a:chOff x="10401300" y="1847850"/>
+          <a:chExt cx="1095375" cy="723900"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="7" name="TextBox 6"/>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="10401300" y="1847850"/>
+            <a:ext cx="1095375" cy="723900"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="lt1"/>
+          </a:solidFill>
+          <a:ln w="9525" cmpd="sng">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100" b="1"/>
+              <a:t>Required</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:endParaRPr lang="en-US" sz="1100" b="1"/>
+          </a:p>
+          <a:p>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100" b="1"/>
+              <a:t>Optional</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="8" name="Rectangle 7"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm flipV="1">
+            <a:off x="11134727" y="1933575"/>
+            <a:ext cx="209548" cy="228600"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:srgbClr val="92D050"/>
+          </a:solidFill>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="9" name="Rectangle 8"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm flipV="1">
+            <a:off x="11134727" y="2266950"/>
+            <a:ext cx="209548" cy="228600"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:srgbClr val="FFC000"/>
+          </a:solidFill>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>952500</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="TextBox 9"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5572125" y="2924175"/>
+          <a:ext cx="3667125" cy="790575"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="92D050"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1"/>
+            <a:t>other_variable</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" baseline="0"/>
+            <a:t> </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" baseline="0"/>
+            <a:t>This column specifies the names of the original select_one or select_multiple questions containing the other choice options.</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="1100" b="0"/>
         </a:p>
@@ -5918,41 +8105,44 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="A8" activeCellId="1" sqref="D20 A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="4" max="4" width="20.7109375" customWidth="1"/>
+    <col min="5" max="5" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
+      <c r="E1" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" s="3"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:D1">
+  <conditionalFormatting sqref="A1:E1">
     <cfRule type="expression" dxfId="23" priority="2">
       <formula>$A1="variable"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:D1048576">
+  <conditionalFormatting sqref="A1:E1048576">
     <cfRule type="expression" dxfId="22" priority="1">
       <formula>$A1&lt;&gt;""</formula>
     </cfRule>
@@ -5966,8 +8156,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15"/>
@@ -5983,16 +8173,16 @@
         <v>9</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -6034,7 +8224,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15"/>
@@ -6044,13 +8234,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E1" s="3"/>
     </row>
@@ -6092,29 +8282,29 @@
   <dimension ref="A1:F89"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="A2" sqref="A2:E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>18</v>
-      </c>
       <c r="E1" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -6348,7 +8538,7 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -6361,7 +8551,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15"/>
@@ -6371,13 +8561,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -6407,7 +8597,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:D6"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15"/>
@@ -6420,10 +8610,10 @@
         <v>7</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -6450,7 +8640,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C10"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15"/>
@@ -6460,10 +8650,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -6514,41 +8704,47 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
-    </row>
-    <row r="3" spans="1:3">
+      <c r="D1" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="B3" s="3"/>
-    </row>
-    <row r="5" spans="1:3">
+      <c r="C3" s="3"/>
+    </row>
+    <row r="5" spans="1:4">
       <c r="B5" s="3"/>
-    </row>
-    <row r="7" spans="1:3">
+      <c r="C5" s="3"/>
+    </row>
+    <row r="7" spans="1:4">
       <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:C1">
+  <conditionalFormatting sqref="A1:D1">
     <cfRule type="expression" dxfId="15" priority="2">
       <formula>$A1="variable"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:C1048576">
+  <conditionalFormatting sqref="A1:D1048576">
     <cfRule type="expression" dxfId="14" priority="1">
       <formula>$A1&lt;&gt;""</formula>
     </cfRule>
@@ -6563,7 +8759,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15"/>
@@ -6573,16 +8769,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>19</v>
-      </c>
       <c r="E1" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -6626,635 +8822,552 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C602"/>
+  <dimension ref="A1:B602"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="C2" s="3"/>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="C4" s="3"/>
-    </row>
-    <row r="15" spans="1:3">
+    </row>
+    <row r="2" spans="1:2">
+      <c r="B2" s="3"/>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="B4" s="3"/>
+    </row>
+    <row r="15" spans="1:2">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-    </row>
-    <row r="16" spans="1:3">
+    </row>
+    <row r="16" spans="1:2">
       <c r="A16" s="3"/>
-      <c r="B16" s="3"/>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="C17" s="3"/>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="C19" s="3"/>
-    </row>
-    <row r="30" spans="1:3">
+    </row>
+    <row r="17" spans="1:2">
+      <c r="B17" s="3"/>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="B19" s="3"/>
+    </row>
+    <row r="30" spans="1:2">
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
-      <c r="C30" s="3"/>
-    </row>
-    <row r="31" spans="1:3">
+    </row>
+    <row r="31" spans="1:2">
       <c r="A31" s="3"/>
-      <c r="B31" s="3"/>
-    </row>
-    <row r="32" spans="1:3">
-      <c r="C32" s="3"/>
-    </row>
-    <row r="34" spans="1:3">
-      <c r="C34" s="3"/>
-    </row>
-    <row r="45" spans="1:3">
+    </row>
+    <row r="32" spans="1:2">
+      <c r="B32" s="3"/>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="B34" s="3"/>
+    </row>
+    <row r="45" spans="1:2">
       <c r="A45" s="3"/>
       <c r="B45" s="3"/>
-      <c r="C45" s="3"/>
-    </row>
-    <row r="46" spans="1:3">
+    </row>
+    <row r="46" spans="1:2">
       <c r="A46" s="3"/>
-      <c r="B46" s="3"/>
-    </row>
-    <row r="47" spans="1:3">
-      <c r="C47" s="3"/>
-    </row>
-    <row r="49" spans="1:3">
-      <c r="C49" s="3"/>
-    </row>
-    <row r="60" spans="1:3">
+    </row>
+    <row r="47" spans="1:2">
+      <c r="B47" s="3"/>
+    </row>
+    <row r="49" spans="1:2">
+      <c r="B49" s="3"/>
+    </row>
+    <row r="60" spans="1:2">
       <c r="A60" s="3"/>
       <c r="B60" s="3"/>
-      <c r="C60" s="3"/>
-    </row>
-    <row r="61" spans="1:3">
+    </row>
+    <row r="61" spans="1:2">
       <c r="A61" s="3"/>
-      <c r="B61" s="3"/>
-    </row>
-    <row r="62" spans="1:3">
-      <c r="C62" s="3"/>
-    </row>
-    <row r="64" spans="1:3">
-      <c r="C64" s="3"/>
-    </row>
-    <row r="75" spans="1:3">
+    </row>
+    <row r="62" spans="1:2">
+      <c r="B62" s="3"/>
+    </row>
+    <row r="64" spans="1:2">
+      <c r="B64" s="3"/>
+    </row>
+    <row r="75" spans="1:2">
       <c r="A75" s="3"/>
       <c r="B75" s="3"/>
-      <c r="C75" s="3"/>
-    </row>
-    <row r="76" spans="1:3">
+    </row>
+    <row r="76" spans="1:2">
       <c r="A76" s="3"/>
-      <c r="B76" s="3"/>
-    </row>
-    <row r="77" spans="1:3">
-      <c r="C77" s="3"/>
-    </row>
-    <row r="79" spans="1:3">
-      <c r="C79" s="3"/>
-    </row>
-    <row r="90" spans="1:3">
+    </row>
+    <row r="77" spans="1:2">
+      <c r="B77" s="3"/>
+    </row>
+    <row r="79" spans="1:2">
+      <c r="B79" s="3"/>
+    </row>
+    <row r="90" spans="1:2">
       <c r="A90" s="3"/>
       <c r="B90" s="3"/>
-      <c r="C90" s="3"/>
-    </row>
-    <row r="91" spans="1:3">
+    </row>
+    <row r="91" spans="1:2">
       <c r="A91" s="3"/>
-      <c r="B91" s="3"/>
-    </row>
-    <row r="92" spans="1:3">
-      <c r="C92" s="3"/>
-    </row>
-    <row r="94" spans="1:3">
-      <c r="C94" s="3"/>
-    </row>
-    <row r="105" spans="1:3">
+    </row>
+    <row r="92" spans="1:2">
+      <c r="B92" s="3"/>
+    </row>
+    <row r="94" spans="1:2">
+      <c r="B94" s="3"/>
+    </row>
+    <row r="105" spans="1:2">
       <c r="A105" s="3"/>
       <c r="B105" s="3"/>
-      <c r="C105" s="3"/>
-    </row>
-    <row r="106" spans="1:3">
+    </row>
+    <row r="106" spans="1:2">
       <c r="A106" s="3"/>
-      <c r="B106" s="3"/>
-    </row>
-    <row r="107" spans="1:3">
-      <c r="C107" s="3"/>
-    </row>
-    <row r="109" spans="1:3">
-      <c r="C109" s="3"/>
-    </row>
-    <row r="120" spans="1:3">
+    </row>
+    <row r="107" spans="1:2">
+      <c r="B107" s="3"/>
+    </row>
+    <row r="109" spans="1:2">
+      <c r="B109" s="3"/>
+    </row>
+    <row r="120" spans="1:2">
       <c r="A120" s="3"/>
       <c r="B120" s="3"/>
-      <c r="C120" s="3"/>
-    </row>
-    <row r="121" spans="1:3">
+    </row>
+    <row r="121" spans="1:2">
       <c r="A121" s="3"/>
-      <c r="B121" s="3"/>
-    </row>
-    <row r="122" spans="1:3">
-      <c r="C122" s="3"/>
-    </row>
-    <row r="124" spans="1:3">
-      <c r="C124" s="3"/>
-    </row>
-    <row r="135" spans="1:3">
+    </row>
+    <row r="122" spans="1:2">
+      <c r="B122" s="3"/>
+    </row>
+    <row r="124" spans="1:2">
+      <c r="B124" s="3"/>
+    </row>
+    <row r="135" spans="1:2">
       <c r="A135" s="3"/>
       <c r="B135" s="3"/>
-      <c r="C135" s="3"/>
-    </row>
-    <row r="136" spans="1:3">
+    </row>
+    <row r="136" spans="1:2">
       <c r="A136" s="3"/>
-      <c r="B136" s="3"/>
-    </row>
-    <row r="137" spans="1:3">
-      <c r="C137" s="3"/>
-    </row>
-    <row r="139" spans="1:3">
-      <c r="C139" s="3"/>
-    </row>
-    <row r="150" spans="1:3">
+    </row>
+    <row r="137" spans="1:2">
+      <c r="B137" s="3"/>
+    </row>
+    <row r="139" spans="1:2">
+      <c r="B139" s="3"/>
+    </row>
+    <row r="150" spans="1:2">
       <c r="A150" s="3"/>
       <c r="B150" s="3"/>
-      <c r="C150" s="3"/>
-    </row>
-    <row r="151" spans="1:3">
+    </row>
+    <row r="151" spans="1:2">
       <c r="A151" s="3"/>
-      <c r="B151" s="3"/>
-    </row>
-    <row r="152" spans="1:3">
-      <c r="C152" s="3"/>
-    </row>
-    <row r="154" spans="1:3">
-      <c r="C154" s="3"/>
-    </row>
-    <row r="165" spans="1:3">
+    </row>
+    <row r="152" spans="1:2">
+      <c r="B152" s="3"/>
+    </row>
+    <row r="154" spans="1:2">
+      <c r="B154" s="3"/>
+    </row>
+    <row r="165" spans="1:2">
       <c r="A165" s="3"/>
       <c r="B165" s="3"/>
-      <c r="C165" s="3"/>
-    </row>
-    <row r="166" spans="1:3">
+    </row>
+    <row r="166" spans="1:2">
       <c r="A166" s="3"/>
-      <c r="B166" s="3"/>
-    </row>
-    <row r="167" spans="1:3">
-      <c r="C167" s="3"/>
-    </row>
-    <row r="169" spans="1:3">
-      <c r="C169" s="3"/>
-    </row>
-    <row r="180" spans="1:3">
+    </row>
+    <row r="167" spans="1:2">
+      <c r="B167" s="3"/>
+    </row>
+    <row r="169" spans="1:2">
+      <c r="B169" s="3"/>
+    </row>
+    <row r="180" spans="1:2">
       <c r="A180" s="3"/>
       <c r="B180" s="3"/>
-      <c r="C180" s="3"/>
-    </row>
-    <row r="181" spans="1:3">
+    </row>
+    <row r="181" spans="1:2">
       <c r="A181" s="3"/>
-      <c r="B181" s="3"/>
-    </row>
-    <row r="182" spans="1:3">
-      <c r="C182" s="3"/>
-    </row>
-    <row r="184" spans="1:3">
-      <c r="C184" s="3"/>
-    </row>
-    <row r="195" spans="1:3">
+    </row>
+    <row r="182" spans="1:2">
+      <c r="B182" s="3"/>
+    </row>
+    <row r="184" spans="1:2">
+      <c r="B184" s="3"/>
+    </row>
+    <row r="195" spans="1:2">
       <c r="A195" s="3"/>
       <c r="B195" s="3"/>
-      <c r="C195" s="3"/>
-    </row>
-    <row r="196" spans="1:3">
+    </row>
+    <row r="196" spans="1:2">
       <c r="A196" s="3"/>
-      <c r="B196" s="3"/>
-    </row>
-    <row r="197" spans="1:3">
-      <c r="C197" s="3"/>
-    </row>
-    <row r="199" spans="1:3">
-      <c r="C199" s="3"/>
-    </row>
-    <row r="210" spans="1:3">
+    </row>
+    <row r="197" spans="1:2">
+      <c r="B197" s="3"/>
+    </row>
+    <row r="199" spans="1:2">
+      <c r="B199" s="3"/>
+    </row>
+    <row r="210" spans="1:2">
       <c r="A210" s="3"/>
       <c r="B210" s="3"/>
-      <c r="C210" s="3"/>
-    </row>
-    <row r="211" spans="1:3">
+    </row>
+    <row r="211" spans="1:2">
       <c r="A211" s="3"/>
-      <c r="B211" s="3"/>
-    </row>
-    <row r="212" spans="1:3">
-      <c r="C212" s="3"/>
-    </row>
-    <row r="214" spans="1:3">
-      <c r="C214" s="3"/>
-    </row>
-    <row r="225" spans="1:3">
+    </row>
+    <row r="212" spans="1:2">
+      <c r="B212" s="3"/>
+    </row>
+    <row r="214" spans="1:2">
+      <c r="B214" s="3"/>
+    </row>
+    <row r="225" spans="1:2">
       <c r="A225" s="3"/>
       <c r="B225" s="3"/>
-      <c r="C225" s="3"/>
-    </row>
-    <row r="226" spans="1:3">
+    </row>
+    <row r="226" spans="1:2">
       <c r="A226" s="3"/>
-      <c r="B226" s="3"/>
-    </row>
-    <row r="227" spans="1:3">
-      <c r="C227" s="3"/>
-    </row>
-    <row r="229" spans="1:3">
-      <c r="C229" s="3"/>
-    </row>
-    <row r="240" spans="1:3">
+    </row>
+    <row r="227" spans="1:2">
+      <c r="B227" s="3"/>
+    </row>
+    <row r="229" spans="1:2">
+      <c r="B229" s="3"/>
+    </row>
+    <row r="240" spans="1:2">
       <c r="A240" s="3"/>
       <c r="B240" s="3"/>
-      <c r="C240" s="3"/>
-    </row>
-    <row r="241" spans="1:3">
+    </row>
+    <row r="241" spans="1:2">
       <c r="A241" s="3"/>
-      <c r="B241" s="3"/>
-    </row>
-    <row r="242" spans="1:3">
-      <c r="C242" s="3"/>
-    </row>
-    <row r="244" spans="1:3">
-      <c r="C244" s="3"/>
-    </row>
-    <row r="255" spans="1:3">
+    </row>
+    <row r="242" spans="1:2">
+      <c r="B242" s="3"/>
+    </row>
+    <row r="244" spans="1:2">
+      <c r="B244" s="3"/>
+    </row>
+    <row r="255" spans="1:2">
       <c r="A255" s="3"/>
       <c r="B255" s="3"/>
-      <c r="C255" s="3"/>
-    </row>
-    <row r="256" spans="1:3">
+    </row>
+    <row r="256" spans="1:2">
       <c r="A256" s="3"/>
-      <c r="B256" s="3"/>
-    </row>
-    <row r="257" spans="1:3">
-      <c r="C257" s="3"/>
-    </row>
-    <row r="259" spans="1:3">
-      <c r="C259" s="3"/>
-    </row>
-    <row r="270" spans="1:3">
+    </row>
+    <row r="257" spans="1:2">
+      <c r="B257" s="3"/>
+    </row>
+    <row r="259" spans="1:2">
+      <c r="B259" s="3"/>
+    </row>
+    <row r="270" spans="1:2">
       <c r="A270" s="3"/>
       <c r="B270" s="3"/>
-      <c r="C270" s="3"/>
-    </row>
-    <row r="271" spans="1:3">
+    </row>
+    <row r="271" spans="1:2">
       <c r="A271" s="3"/>
-      <c r="B271" s="3"/>
-    </row>
-    <row r="272" spans="1:3">
-      <c r="C272" s="3"/>
-    </row>
-    <row r="274" spans="1:3">
-      <c r="C274" s="3"/>
-    </row>
-    <row r="285" spans="1:3">
+    </row>
+    <row r="272" spans="1:2">
+      <c r="B272" s="3"/>
+    </row>
+    <row r="274" spans="1:2">
+      <c r="B274" s="3"/>
+    </row>
+    <row r="285" spans="1:2">
       <c r="A285" s="3"/>
       <c r="B285" s="3"/>
-      <c r="C285" s="3"/>
-    </row>
-    <row r="286" spans="1:3">
+    </row>
+    <row r="286" spans="1:2">
       <c r="A286" s="3"/>
-      <c r="B286" s="3"/>
-    </row>
-    <row r="287" spans="1:3">
-      <c r="C287" s="3"/>
-    </row>
-    <row r="289" spans="1:3">
-      <c r="C289" s="3"/>
-    </row>
-    <row r="300" spans="1:3">
+    </row>
+    <row r="287" spans="1:2">
+      <c r="B287" s="3"/>
+    </row>
+    <row r="289" spans="1:2">
+      <c r="B289" s="3"/>
+    </row>
+    <row r="300" spans="1:2">
       <c r="A300" s="3"/>
       <c r="B300" s="3"/>
-      <c r="C300" s="3"/>
-    </row>
-    <row r="301" spans="1:3">
+    </row>
+    <row r="301" spans="1:2">
       <c r="A301" s="3"/>
-      <c r="B301" s="3"/>
-    </row>
-    <row r="302" spans="1:3">
-      <c r="C302" s="3"/>
-    </row>
-    <row r="304" spans="1:3">
-      <c r="C304" s="3"/>
-    </row>
-    <row r="315" spans="1:3">
+    </row>
+    <row r="302" spans="1:2">
+      <c r="B302" s="3"/>
+    </row>
+    <row r="304" spans="1:2">
+      <c r="B304" s="3"/>
+    </row>
+    <row r="315" spans="1:2">
       <c r="A315" s="3"/>
       <c r="B315" s="3"/>
-      <c r="C315" s="3"/>
-    </row>
-    <row r="316" spans="1:3">
+    </row>
+    <row r="316" spans="1:2">
       <c r="A316" s="3"/>
-      <c r="B316" s="3"/>
-    </row>
-    <row r="317" spans="1:3">
-      <c r="C317" s="3"/>
-    </row>
-    <row r="319" spans="1:3">
-      <c r="C319" s="3"/>
-    </row>
-    <row r="330" spans="1:3">
+    </row>
+    <row r="317" spans="1:2">
+      <c r="B317" s="3"/>
+    </row>
+    <row r="319" spans="1:2">
+      <c r="B319" s="3"/>
+    </row>
+    <row r="330" spans="1:2">
       <c r="A330" s="3"/>
       <c r="B330" s="3"/>
-      <c r="C330" s="3"/>
-    </row>
-    <row r="331" spans="1:3">
+    </row>
+    <row r="331" spans="1:2">
       <c r="A331" s="3"/>
-      <c r="B331" s="3"/>
-    </row>
-    <row r="332" spans="1:3">
-      <c r="C332" s="3"/>
-    </row>
-    <row r="334" spans="1:3">
-      <c r="C334" s="3"/>
-    </row>
-    <row r="345" spans="1:3">
+    </row>
+    <row r="332" spans="1:2">
+      <c r="B332" s="3"/>
+    </row>
+    <row r="334" spans="1:2">
+      <c r="B334" s="3"/>
+    </row>
+    <row r="345" spans="1:2">
       <c r="A345" s="3"/>
       <c r="B345" s="3"/>
-      <c r="C345" s="3"/>
-    </row>
-    <row r="346" spans="1:3">
+    </row>
+    <row r="346" spans="1:2">
       <c r="A346" s="3"/>
-      <c r="B346" s="3"/>
-    </row>
-    <row r="347" spans="1:3">
-      <c r="C347" s="3"/>
-    </row>
-    <row r="349" spans="1:3">
-      <c r="C349" s="3"/>
-    </row>
-    <row r="360" spans="1:3">
+    </row>
+    <row r="347" spans="1:2">
+      <c r="B347" s="3"/>
+    </row>
+    <row r="349" spans="1:2">
+      <c r="B349" s="3"/>
+    </row>
+    <row r="360" spans="1:2">
       <c r="A360" s="3"/>
       <c r="B360" s="3"/>
-      <c r="C360" s="3"/>
-    </row>
-    <row r="361" spans="1:3">
+    </row>
+    <row r="361" spans="1:2">
       <c r="A361" s="3"/>
-      <c r="B361" s="3"/>
-    </row>
-    <row r="362" spans="1:3">
-      <c r="C362" s="3"/>
-    </row>
-    <row r="364" spans="1:3">
-      <c r="C364" s="3"/>
-    </row>
-    <row r="375" spans="1:3">
+    </row>
+    <row r="362" spans="1:2">
+      <c r="B362" s="3"/>
+    </row>
+    <row r="364" spans="1:2">
+      <c r="B364" s="3"/>
+    </row>
+    <row r="375" spans="1:2">
       <c r="A375" s="3"/>
       <c r="B375" s="3"/>
-      <c r="C375" s="3"/>
-    </row>
-    <row r="376" spans="1:3">
+    </row>
+    <row r="376" spans="1:2">
       <c r="A376" s="3"/>
-      <c r="B376" s="3"/>
-    </row>
-    <row r="377" spans="1:3">
-      <c r="C377" s="3"/>
-    </row>
-    <row r="379" spans="1:3">
-      <c r="C379" s="3"/>
-    </row>
-    <row r="390" spans="1:3">
+    </row>
+    <row r="377" spans="1:2">
+      <c r="B377" s="3"/>
+    </row>
+    <row r="379" spans="1:2">
+      <c r="B379" s="3"/>
+    </row>
+    <row r="390" spans="1:2">
       <c r="A390" s="3"/>
       <c r="B390" s="3"/>
-      <c r="C390" s="3"/>
-    </row>
-    <row r="391" spans="1:3">
+    </row>
+    <row r="391" spans="1:2">
       <c r="A391" s="3"/>
-      <c r="B391" s="3"/>
-    </row>
-    <row r="392" spans="1:3">
-      <c r="C392" s="3"/>
-    </row>
-    <row r="394" spans="1:3">
-      <c r="C394" s="3"/>
-    </row>
-    <row r="405" spans="1:3">
+    </row>
+    <row r="392" spans="1:2">
+      <c r="B392" s="3"/>
+    </row>
+    <row r="394" spans="1:2">
+      <c r="B394" s="3"/>
+    </row>
+    <row r="405" spans="1:2">
       <c r="A405" s="3"/>
       <c r="B405" s="3"/>
-      <c r="C405" s="3"/>
-    </row>
-    <row r="406" spans="1:3">
+    </row>
+    <row r="406" spans="1:2">
       <c r="A406" s="3"/>
-      <c r="B406" s="3"/>
-    </row>
-    <row r="407" spans="1:3">
-      <c r="C407" s="3"/>
-    </row>
-    <row r="409" spans="1:3">
-      <c r="C409" s="3"/>
-    </row>
-    <row r="420" spans="1:3">
+    </row>
+    <row r="407" spans="1:2">
+      <c r="B407" s="3"/>
+    </row>
+    <row r="409" spans="1:2">
+      <c r="B409" s="3"/>
+    </row>
+    <row r="420" spans="1:2">
       <c r="A420" s="3"/>
       <c r="B420" s="3"/>
-      <c r="C420" s="3"/>
-    </row>
-    <row r="421" spans="1:3">
+    </row>
+    <row r="421" spans="1:2">
       <c r="A421" s="3"/>
-      <c r="B421" s="3"/>
-    </row>
-    <row r="422" spans="1:3">
-      <c r="C422" s="3"/>
-    </row>
-    <row r="424" spans="1:3">
-      <c r="C424" s="3"/>
-    </row>
-    <row r="435" spans="1:3">
+    </row>
+    <row r="422" spans="1:2">
+      <c r="B422" s="3"/>
+    </row>
+    <row r="424" spans="1:2">
+      <c r="B424" s="3"/>
+    </row>
+    <row r="435" spans="1:2">
       <c r="A435" s="3"/>
       <c r="B435" s="3"/>
-      <c r="C435" s="3"/>
-    </row>
-    <row r="436" spans="1:3">
+    </row>
+    <row r="436" spans="1:2">
       <c r="A436" s="3"/>
-      <c r="B436" s="3"/>
-    </row>
-    <row r="437" spans="1:3">
-      <c r="C437" s="3"/>
-    </row>
-    <row r="439" spans="1:3">
-      <c r="C439" s="3"/>
-    </row>
-    <row r="450" spans="1:3">
+    </row>
+    <row r="437" spans="1:2">
+      <c r="B437" s="3"/>
+    </row>
+    <row r="439" spans="1:2">
+      <c r="B439" s="3"/>
+    </row>
+    <row r="450" spans="1:2">
       <c r="A450" s="3"/>
       <c r="B450" s="3"/>
-      <c r="C450" s="3"/>
-    </row>
-    <row r="451" spans="1:3">
+    </row>
+    <row r="451" spans="1:2">
       <c r="A451" s="3"/>
-      <c r="B451" s="3"/>
-    </row>
-    <row r="452" spans="1:3">
-      <c r="C452" s="3"/>
-    </row>
-    <row r="454" spans="1:3">
-      <c r="C454" s="3"/>
-    </row>
-    <row r="465" spans="1:3">
+    </row>
+    <row r="452" spans="1:2">
+      <c r="B452" s="3"/>
+    </row>
+    <row r="454" spans="1:2">
+      <c r="B454" s="3"/>
+    </row>
+    <row r="465" spans="1:2">
       <c r="A465" s="3"/>
       <c r="B465" s="3"/>
-      <c r="C465" s="3"/>
-    </row>
-    <row r="466" spans="1:3">
+    </row>
+    <row r="466" spans="1:2">
       <c r="A466" s="3"/>
-      <c r="B466" s="3"/>
-    </row>
-    <row r="467" spans="1:3">
-      <c r="C467" s="3"/>
-    </row>
-    <row r="469" spans="1:3">
-      <c r="C469" s="3"/>
-    </row>
-    <row r="480" spans="1:3">
+    </row>
+    <row r="467" spans="1:2">
+      <c r="B467" s="3"/>
+    </row>
+    <row r="469" spans="1:2">
+      <c r="B469" s="3"/>
+    </row>
+    <row r="480" spans="1:2">
       <c r="A480" s="3"/>
       <c r="B480" s="3"/>
-      <c r="C480" s="3"/>
-    </row>
-    <row r="481" spans="1:3">
+    </row>
+    <row r="481" spans="1:2">
       <c r="A481" s="3"/>
-      <c r="B481" s="3"/>
-    </row>
-    <row r="482" spans="1:3">
-      <c r="C482" s="3"/>
-    </row>
-    <row r="484" spans="1:3">
-      <c r="C484" s="3"/>
-    </row>
-    <row r="495" spans="1:3">
+    </row>
+    <row r="482" spans="1:2">
+      <c r="B482" s="3"/>
+    </row>
+    <row r="484" spans="1:2">
+      <c r="B484" s="3"/>
+    </row>
+    <row r="495" spans="1:2">
       <c r="A495" s="3"/>
       <c r="B495" s="3"/>
-      <c r="C495" s="3"/>
-    </row>
-    <row r="496" spans="1:3">
+    </row>
+    <row r="496" spans="1:2">
       <c r="A496" s="3"/>
-      <c r="B496" s="3"/>
-    </row>
-    <row r="497" spans="1:3">
-      <c r="C497" s="3"/>
-    </row>
-    <row r="499" spans="1:3">
-      <c r="C499" s="3"/>
-    </row>
-    <row r="510" spans="1:3">
+    </row>
+    <row r="497" spans="1:2">
+      <c r="B497" s="3"/>
+    </row>
+    <row r="499" spans="1:2">
+      <c r="B499" s="3"/>
+    </row>
+    <row r="510" spans="1:2">
       <c r="A510" s="3"/>
       <c r="B510" s="3"/>
-      <c r="C510" s="3"/>
-    </row>
-    <row r="511" spans="1:3">
+    </row>
+    <row r="511" spans="1:2">
       <c r="A511" s="3"/>
-      <c r="B511" s="3"/>
-    </row>
-    <row r="512" spans="1:3">
-      <c r="C512" s="3"/>
-    </row>
-    <row r="514" spans="1:3">
-      <c r="C514" s="3"/>
-    </row>
-    <row r="525" spans="1:3">
+    </row>
+    <row r="512" spans="1:2">
+      <c r="B512" s="3"/>
+    </row>
+    <row r="514" spans="1:2">
+      <c r="B514" s="3"/>
+    </row>
+    <row r="525" spans="1:2">
       <c r="A525" s="3"/>
       <c r="B525" s="3"/>
-      <c r="C525" s="3"/>
-    </row>
-    <row r="526" spans="1:3">
+    </row>
+    <row r="526" spans="1:2">
       <c r="A526" s="3"/>
-      <c r="B526" s="3"/>
-    </row>
-    <row r="527" spans="1:3">
-      <c r="C527" s="3"/>
-    </row>
-    <row r="529" spans="1:3">
-      <c r="C529" s="3"/>
-    </row>
-    <row r="540" spans="1:3">
+    </row>
+    <row r="527" spans="1:2">
+      <c r="B527" s="3"/>
+    </row>
+    <row r="529" spans="1:2">
+      <c r="B529" s="3"/>
+    </row>
+    <row r="540" spans="1:2">
       <c r="A540" s="3"/>
       <c r="B540" s="3"/>
-      <c r="C540" s="3"/>
-    </row>
-    <row r="541" spans="1:3">
+    </row>
+    <row r="541" spans="1:2">
       <c r="A541" s="3"/>
-      <c r="B541" s="3"/>
-    </row>
-    <row r="542" spans="1:3">
-      <c r="C542" s="3"/>
-    </row>
-    <row r="544" spans="1:3">
-      <c r="C544" s="3"/>
-    </row>
-    <row r="555" spans="1:3">
+    </row>
+    <row r="542" spans="1:2">
+      <c r="B542" s="3"/>
+    </row>
+    <row r="544" spans="1:2">
+      <c r="B544" s="3"/>
+    </row>
+    <row r="555" spans="1:2">
       <c r="A555" s="3"/>
       <c r="B555" s="3"/>
-      <c r="C555" s="3"/>
-    </row>
-    <row r="556" spans="1:3">
+    </row>
+    <row r="556" spans="1:2">
       <c r="A556" s="3"/>
-      <c r="B556" s="3"/>
-    </row>
-    <row r="557" spans="1:3">
-      <c r="C557" s="3"/>
-    </row>
-    <row r="559" spans="1:3">
-      <c r="C559" s="3"/>
-    </row>
-    <row r="570" spans="1:3">
+    </row>
+    <row r="557" spans="1:2">
+      <c r="B557" s="3"/>
+    </row>
+    <row r="559" spans="1:2">
+      <c r="B559" s="3"/>
+    </row>
+    <row r="570" spans="1:2">
       <c r="A570" s="3"/>
       <c r="B570" s="3"/>
-      <c r="C570" s="3"/>
-    </row>
-    <row r="571" spans="1:3">
+    </row>
+    <row r="571" spans="1:2">
       <c r="A571" s="3"/>
-      <c r="B571" s="3"/>
-    </row>
-    <row r="572" spans="1:3">
-      <c r="C572" s="3"/>
-    </row>
-    <row r="574" spans="1:3">
-      <c r="C574" s="3"/>
-    </row>
-    <row r="585" spans="1:3">
+    </row>
+    <row r="572" spans="1:2">
+      <c r="B572" s="3"/>
+    </row>
+    <row r="574" spans="1:2">
+      <c r="B574" s="3"/>
+    </row>
+    <row r="585" spans="1:2">
       <c r="A585" s="3"/>
       <c r="B585" s="3"/>
-      <c r="C585" s="3"/>
-    </row>
-    <row r="586" spans="1:3">
+    </row>
+    <row r="586" spans="1:2">
       <c r="A586" s="3"/>
-      <c r="B586" s="3"/>
-    </row>
-    <row r="587" spans="1:3">
-      <c r="C587" s="3"/>
-    </row>
-    <row r="589" spans="1:3">
-      <c r="C589" s="3"/>
-    </row>
-    <row r="600" spans="1:3">
+    </row>
+    <row r="587" spans="1:2">
+      <c r="B587" s="3"/>
+    </row>
+    <row r="589" spans="1:2">
+      <c r="B589" s="3"/>
+    </row>
+    <row r="600" spans="1:2">
       <c r="A600" s="3"/>
       <c r="B600" s="3"/>
-      <c r="C600" s="3"/>
-    </row>
-    <row r="601" spans="1:3">
+    </row>
+    <row r="601" spans="1:2">
       <c r="A601" s="3"/>
-      <c r="B601" s="3"/>
-    </row>
-    <row r="602" spans="1:3">
-      <c r="C602" s="3"/>
+    </row>
+    <row r="602" spans="1:2">
+      <c r="B602" s="3"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:C1">
+  <conditionalFormatting sqref="A1:B1">
     <cfRule type="expression" dxfId="11" priority="3">
       <formula>$A1="variable"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:C1048576">
+  <conditionalFormatting sqref="A1:B1048576">
     <cfRule type="expression" dxfId="10" priority="2">
       <formula>$A1&lt;&gt;""</formula>
     </cfRule>
@@ -7268,8 +9381,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G72"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15"/>
@@ -7291,10 +9404,10 @@
         <v>6</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -7780,82 +9893,93 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="D1" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
-    </row>
-    <row r="3" spans="1:3">
+      <c r="C2" s="3"/>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" s="3"/>
-      <c r="C3" s="3"/>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="C5" s="3"/>
-    </row>
-    <row r="7" spans="1:3">
+      <c r="B3" s="3"/>
+      <c r="D3" s="3"/>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="D5" s="3"/>
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
-    </row>
-    <row r="8" spans="1:3">
+      <c r="D7" s="3"/>
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="C9" s="3"/>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="C11" s="3"/>
-    </row>
-    <row r="13" spans="1:3">
+      <c r="C8" s="3"/>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="D9" s="3"/>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="D11" s="3"/>
+    </row>
+    <row r="13" spans="1:4">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
-    </row>
-    <row r="14" spans="1:3">
+      <c r="D13" s="3"/>
+    </row>
+    <row r="14" spans="1:4">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="C15" s="3"/>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="C17" s="3"/>
-    </row>
-    <row r="19" spans="1:3">
+      <c r="C14" s="3"/>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="D15" s="3"/>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="D17" s="3"/>
+    </row>
+    <row r="19" spans="1:4">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
-    </row>
-    <row r="20" spans="1:3">
+      <c r="D19" s="3"/>
+    </row>
+    <row r="20" spans="1:4">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:C1">
+  <conditionalFormatting sqref="A1:D1">
     <cfRule type="expression" dxfId="7" priority="2">
       <formula>$A1="specify_variable"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:C1048576">
+  <conditionalFormatting sqref="A1:D1048576">
     <cfRule type="expression" dxfId="6" priority="1">
       <formula>$A1&lt;&gt;""</formula>
     </cfRule>

</xml_diff>

<commit_message>
Allows multiple variables per check in check 6; changes check 6 instructions in input sheet.
</commit_message>
<xml_diff>
--- a/xlsx/hfc_inputs_blank.xlsx
+++ b/xlsx/hfc_inputs_blank.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cboyer.IPA\Desktop\high-frequency-checks\exercise\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\HFCCode\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11970" windowHeight="4650" firstSheet="2" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11970" windowHeight="4650" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="1. incomplete" sheetId="1" r:id="rId1"/>
@@ -123,7 +123,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -5422,15 +5422,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>57150</xdr:colOff>
+      <xdr:colOff>66675</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>47624</xdr:rowOff>
+      <xdr:rowOff>123824</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>942975</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>19049</xdr:rowOff>
+      <xdr:colOff>952500</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -5439,8 +5439,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6962775" y="47624"/>
-          <a:ext cx="3648075" cy="1495425"/>
+          <a:off x="6972300" y="123824"/>
+          <a:ext cx="3648075" cy="1828801"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5488,13 +5488,26 @@
           </a:r>
         </a:p>
         <a:p>
-          <a:endParaRPr lang="en-US" sz="1100" b="1" baseline="0"/>
+          <a:endParaRPr lang="en-US" sz="1100" b="0" i="1" baseline="0"/>
         </a:p>
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1100" b="0" i="1" baseline="0"/>
-            <a:t>This check verifies certain skip patterns and survey logic are obeyed. If the survey is properly programmed and tested using SurveyCTO, there should be no violations. However, we include these checks to help identify programming errors or to check for logic added after the survey start.</a:t>
-          </a:r>
+            <a:t>This check verifies that skip patterns and survey logic are being obeyed. This check can test for logic added after the survey start. It can also flag soft checks that should be confirmed by enumerators, such as a household that reports paying school fees but has no children. </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="1" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Patterns that are already enforced by the SurveyCTO form's programming do not need to be included. </a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="0" i="1" baseline="0"/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -5503,15 +5516,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>962025</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:colOff>971550</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -5520,8 +5533,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6962775" y="1676400"/>
-          <a:ext cx="3667125" cy="600075"/>
+          <a:off x="6972300" y="2066925"/>
+          <a:ext cx="3667125" cy="828675"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5567,7 +5580,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1100" b="0" baseline="0"/>
-            <a:t>This column specifies the name of the survey status variable. </a:t>
+            <a:t>This column specifies the names of the variables that are important for the logic test (e.g. children schoolfee). Multiple variables can be entered if separated by a space.</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="1100" b="0"/>
         </a:p>
@@ -5578,15 +5591,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>962025</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:colOff>971550</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -5595,7 +5608,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6962775" y="2343150"/>
+          <a:off x="6972300" y="2952750"/>
           <a:ext cx="3667125" cy="609600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -5639,7 +5652,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1100" b="0" baseline="0"/>
-            <a:t>This column specifies a condition which should evaluate to true (e.g. sex == 1).</a:t>
+            <a:t>This column specifies a condition which should evaluate to true (e.g. children &gt; 0).</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="1100" b="0"/>
         </a:p>
@@ -5650,15 +5663,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>962025</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:colOff>971550</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -5667,7 +5680,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6962775" y="3733800"/>
+          <a:off x="6972300" y="4343400"/>
           <a:ext cx="3667125" cy="609600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -5738,15 +5751,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>962025</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:colOff>971550</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -5755,7 +5768,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6962775" y="4429125"/>
+          <a:off x="6972300" y="5038725"/>
           <a:ext cx="3667125" cy="609600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -5799,7 +5812,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1100" b="0" baseline="0"/>
-            <a:t>This column is not used by Stata, rather it is included for the user's convenience to keep notes about inputs</a:t>
+            <a:t>This column is not used by Stata, rather it is included for the user's convenience to keep notes about inputs.</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="1100" b="0"/>
         </a:p>
@@ -5810,15 +5823,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>962025</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:colOff>971550</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -5827,14 +5840,14 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6962775" y="3038475"/>
+          <a:off x="6972300" y="3648075"/>
           <a:ext cx="3667125" cy="609600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
         <a:solidFill>
-          <a:srgbClr val="92D050"/>
+          <a:srgbClr val="FFC000"/>
         </a:solidFill>
         <a:ln w="9525" cmpd="sng">
           <a:solidFill>
@@ -5870,7 +5883,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1100" b="0" baseline="0"/>
-            <a:t>This column specifies a condition under which the assertion should be true (e.g. pregnant == 1)</a:t>
+            <a:t>This column specifies a condition under which the assertion should be true (e.g. schoolfee &gt; 0).</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="1100" b="0"/>
         </a:p>
@@ -7918,6 +7931,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -7953,6 +7983,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -8758,8 +8805,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15"/>
@@ -9381,7 +9428,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G72"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
@@ -9895,7 +9942,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>

</xml_diff>